<commit_message>
Cambios en el back
</commit_message>
<xml_diff>
--- a/back-end/estudiantes.xlsx
+++ b/back-end/estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhunior\Desktop\ProyectoBaseDatos\proyecto-base-datos\back-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FF5818-0BD9-4D42-9246-D7F3BC5FEEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D83F249-99A7-4FD2-BFAD-21B5D3A7BB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="11808" xr2:uid="{4E3B6DDF-B402-4654-B968-21DF4C067117}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E3B6DDF-B402-4654-B968-21DF4C067117}"/>
   </bookViews>
   <sheets>
     <sheet name="ListaEstudiantes" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -133,11 +133,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -146,7 +196,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -463,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E39C7B-6F59-4854-B3BB-D62E49374EFA}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +541,7 @@
     <col min="4" max="4" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -486,14 +551,16 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>73332032</v>
       </c>
@@ -503,14 +570,16 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>37168</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>69583654</v>
       </c>
@@ -520,14 +589,16 @@
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6">
         <v>36652</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>48856952</v>
       </c>
@@ -537,14 +608,16 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="6">
         <v>37424</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>58456958</v>
       </c>
@@ -554,14 +627,16 @@
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>36950</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F7" s="1"/>
     </row>
   </sheetData>

</xml_diff>